<commit_message>
updated feasible set and added inputs
</commit_message>
<xml_diff>
--- a/example/adducts.xlsx
+++ b/example/adducts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longd\OneDrive - The University of Auckland\Documents\UoA Research\MS_Research\MS-Binding-Sites-Identification\Data\Compound Constraints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longd\OneDrive - The University of Auckland\Documents\UoA Research\MS_Research\MS-Binding-Sites-Identification\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDE0938-9520-4675-AD42-B066335251C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1611C9F-BE98-44C4-9030-1490EC559BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3EA2E049-0DEA-481B-8C40-EB3E0F20B6A8}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
@@ -717,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>

</xml_diff>